<commit_message>
Přidány logovací interfaci a implementovaný věci z dokumentace. Kontrolery checkují permise
</commit_message>
<xml_diff>
--- a/timeline/2M Project Timeline.xlsx
+++ b/timeline/2M Project Timeline.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E376D5-5A39-4278-897B-93D296147E4F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,8 +27,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>lukx</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{A60C1221-C27F-4AAB-A54F-CA08670E1EF3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>lukx:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pro daemona</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{3A75C4DB-E83E-4507-AF1E-02789A1038AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>lukx:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pro admina</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="45">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -54,6 +113,114 @@
   </si>
   <si>
     <t>Task:</t>
+  </si>
+  <si>
+    <t>Vynecháno</t>
+  </si>
+  <si>
+    <t>FTP a SFTP</t>
+  </si>
+  <si>
+    <t>Crash Report daemona</t>
+  </si>
+  <si>
+    <t>Optimializace daemona</t>
+  </si>
+  <si>
+    <t>Druhy zipování</t>
+  </si>
+  <si>
+    <t>Server eviduje přítomnost a up time</t>
+  </si>
+  <si>
+    <t>Pokročile D. logy</t>
+  </si>
+  <si>
+    <t>Pokročile A. logy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Copy card URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Convert to issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Convert note to issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Convert to issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Edit note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Delete note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Vytvořit differential a incremental druhy zaloh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Vytvořit differential a incremental druhy zaloh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Added by lukx1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Edit note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Save note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Press enter to move this card</t>
+  </si>
+  <si>
+    <t>Server maily basic</t>
+  </si>
+  <si>
+    <t>Růža</t>
+  </si>
+  <si>
+    <t>Rambo</t>
+  </si>
+  <si>
+    <t>Lukáš</t>
+  </si>
+  <si>
+    <t>Lukáš a Rambo</t>
+  </si>
+  <si>
+    <t>Možnosti nastavení reportů</t>
+  </si>
+  <si>
+    <t>Rambo a Lukáš</t>
+  </si>
+  <si>
+    <t>Nezaznamenáno</t>
   </si>
 </sst>
 </file>
@@ -64,7 +231,7 @@
     <numFmt numFmtId="164" formatCode="d"/>
     <numFmt numFmtId="165" formatCode="mmm"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -115,8 +282,28 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,8 +340,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -211,6 +428,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -239,7 +467,7 @@
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -320,6 +548,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -565,15 +811,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AF28"/>
+  <dimension ref="B1:AJ125"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1032,21 +1278,25 @@
       <c r="AE7" s="22"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="19"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
+      <c r="B8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="6"/>
       <c r="S8" s="5"/>
@@ -1064,7 +1314,9 @@
       <c r="AE8" s="20"/>
     </row>
     <row r="9" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="19"/>
+      <c r="B9" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
@@ -1079,24 +1331,30 @@
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="20"/>
+      <c r="Q9" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="31"/>
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="31"/>
+      <c r="AC9" s="31"/>
+      <c r="AD9" s="31"/>
+      <c r="AE9" s="32" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
+      <c r="B10" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
@@ -1111,24 +1369,28 @@
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="6"/>
+      <c r="Q10" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28"/>
       <c r="AE10" s="20"/>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="19"/>
+      <c r="B11" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
@@ -1143,10 +1405,12 @@
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="6"/>
+      <c r="Q11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
       <c r="W11" s="5"/>
@@ -1160,7 +1424,9 @@
       <c r="AE11" s="20"/>
     </row>
     <row r="12" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="19"/>
+      <c r="B12" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
@@ -1181,10 +1447,12 @@
       <c r="T12" s="6"/>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="6"/>
+      <c r="W12" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="5"/>
@@ -1192,7 +1460,9 @@
       <c r="AE12" s="20"/>
     </row>
     <row r="13" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="19"/>
+      <c r="B13" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
@@ -1216,15 +1486,19 @@
       <c r="W13" s="5"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="6"/>
+      <c r="Z13" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
       <c r="AE13" s="20"/>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="19"/>
+      <c r="B14" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
@@ -1242,12 +1516,14 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="6"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="5"/>
+      <c r="T14" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
       <c r="Z14" s="6"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="6"/>
@@ -1256,7 +1532,9 @@
       <c r="AE14" s="20"/>
     </row>
     <row r="15" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="19"/>
+      <c r="B15" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
@@ -1271,10 +1549,12 @@
       <c r="N15" s="6"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="6"/>
+      <c r="Q15" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
@@ -1288,7 +1568,9 @@
       <c r="AE15" s="20"/>
     </row>
     <row r="16" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="19"/>
+      <c r="B16" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
@@ -1306,12 +1588,14 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="6"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="5"/>
+      <c r="T16" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
       <c r="Z16" s="6"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="6"/>
@@ -1319,8 +1603,10 @@
       <c r="AD16" s="6"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="19"/>
+    <row r="17" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
@@ -1339,11 +1625,13 @@
       <c r="R17" s="6"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="5"/>
+      <c r="U17" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
       <c r="Z17" s="6"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="6"/>
@@ -1351,7 +1639,7 @@
       <c r="AD17" s="6"/>
       <c r="AE17" s="20"/>
     </row>
-    <row r="18" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -1383,7 +1671,7 @@
       <c r="AD18" s="6"/>
       <c r="AE18" s="20"/>
     </row>
-    <row r="19" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1414,8 +1702,11 @@
       <c r="AC19" s="5"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="20"/>
-    </row>
-    <row r="20" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1446,8 +1737,11 @@
       <c r="AC20" s="5"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="20"/>
-    </row>
-    <row r="21" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1478,8 +1772,11 @@
       <c r="AC21" s="5"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="20"/>
-    </row>
-    <row r="22" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -1510,8 +1807,11 @@
       <c r="AC22" s="5"/>
       <c r="AD22" s="6"/>
       <c r="AE22" s="20"/>
-    </row>
-    <row r="23" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="18"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
@@ -1542,8 +1842,11 @@
       <c r="AC23" s="7"/>
       <c r="AD23" s="8"/>
       <c r="AE23" s="20"/>
-    </row>
-    <row r="24" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="18"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -1574,8 +1877,11 @@
       <c r="AC24" s="5"/>
       <c r="AD24" s="6"/>
       <c r="AE24" s="20"/>
-    </row>
-    <row r="25" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="18"/>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
@@ -1606,8 +1912,11 @@
       <c r="AC25" s="7"/>
       <c r="AD25" s="8"/>
       <c r="AE25" s="20"/>
-    </row>
-    <row r="26" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="18"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -1638,8 +1947,11 @@
       <c r="AC26" s="5"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="20"/>
-    </row>
-    <row r="27" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="18"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
@@ -1670,8 +1982,11 @@
       <c r="AC27" s="7"/>
       <c r="AD27" s="8"/>
       <c r="AE27" s="20"/>
-    </row>
-    <row r="28" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -1702,9 +2017,397 @@
       <c r="AC28" s="5"/>
       <c r="AD28" s="6"/>
       <c r="AE28" s="20"/>
+      <c r="AJ28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ60" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ65" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ69" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ73" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ76" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ77" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ78" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ80" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ81" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ82" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ83" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ84" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ86" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ89" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ90" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ96" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ97" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ98" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ99" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ100" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ101" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ103" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ104" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ105" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ106" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ107" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ108" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ109" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ110" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ112" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ113" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ114" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ115" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ116" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ122" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ123" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="36:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ125" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="17">
+    <mergeCell ref="U17:Y17"/>
+    <mergeCell ref="Q9:AD9"/>
+    <mergeCell ref="W12:Z12"/>
+    <mergeCell ref="T14:Y14"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="T16:Y16"/>
+    <mergeCell ref="C8:P8"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Z13:AD13"/>
+    <mergeCell ref="Q10:AD10"/>
     <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="B1:AE1"/>
     <mergeCell ref="X4:AD4"/>
@@ -1718,7 +2421,7 @@
       <formula>C$7=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="9">
+  <dataValidations disablePrompts="1" count="9">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline in this worksheet. Enter Start Date in cell C2 and other details starting in cell B4" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in cell at right" sqref="B2" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this cell" sqref="C2:E2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
@@ -1738,5 +2441,6 @@
   <ignoredErrors>
     <ignoredError sqref="J5 Q5 X5" formula="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Daemon pozná když server je offline a nehlásí to jako neznámou chybu. Async funkce(CanStart) a její while loop už dávají větší smysl
</commit_message>
<xml_diff>
--- a/timeline/2M Project Timeline.xlsx
+++ b/timeline/2M Project Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426C1EE1-ADA9-4E26-9DEB-7ED466DB8A7C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4F47DA-26AC-49C0-BFBD-33811E4AF066}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Timeline'!$4:$7</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,36 +81,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE15" authorId="0" shapeId="0" xr:uid="{46D1AEBA-5523-478C-8A63-15400303B892}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lukx:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -247,7 +223,7 @@
     <t>Nezaznamenáno</t>
   </si>
   <si>
-    <t>Odloženo</t>
+    <t>Dokončeno</t>
   </si>
 </sst>
 </file>
@@ -258,7 +234,7 @@
     <numFmt numFmtId="164" formatCode="d"/>
     <numFmt numFmtId="165" formatCode="mmm"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -328,19 +304,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -574,6 +537,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -585,27 +569,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -859,7 +822,7 @@
   <dimension ref="B1:AJ125"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9:AD9"/>
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -873,91 +836,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="31">
         <v>43171</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="23" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="25" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="23" t="s">
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="30" t="s">
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -1078,7 +1041,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="30"/>
+      <c r="AE5" s="27"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1197,7 +1160,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="30"/>
+      <c r="AE6" s="27"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1315,7 +1278,7 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43198</v>
       </c>
-      <c r="AE7" s="31"/>
+      <c r="AE7" s="28"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
@@ -1371,22 +1334,22 @@
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="28"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="23"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
       <c r="AE9" s="21" t="s">
         <v>6</v>
       </c>
@@ -1409,22 +1372,22 @@
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="29" t="s">
+      <c r="Q10" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
-      <c r="AB10" s="29"/>
-      <c r="AC10" s="29"/>
-      <c r="AD10" s="29"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="25"/>
       <c r="AE10" s="20"/>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1445,12 +1408,12 @@
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="27" t="s">
+      <c r="Q11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
       <c r="W11" s="5"/>
@@ -1487,12 +1450,12 @@
       <c r="T12" s="6"/>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="32" t="s">
+      <c r="W12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="32"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="5"/>
@@ -1526,13 +1489,13 @@
       <c r="W13" s="5"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="28" t="s">
+      <c r="Z13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="28"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
       <c r="AE13" s="20"/>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1556,14 +1519,14 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="6"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="27" t="s">
+      <c r="T14" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
       <c r="Z14" s="6"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="6"/>
@@ -1589,12 +1552,12 @@
       <c r="N15" s="6"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="32" t="s">
+      <c r="Q15" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
@@ -1630,14 +1593,14 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="6"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="29" t="s">
+      <c r="T16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
       <c r="Z16" s="6"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="6"/>
@@ -1667,19 +1630,21 @@
       <c r="R17" s="6"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="32" t="s">
+      <c r="U17" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="32"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
       <c r="Z17" s="6"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="6"/>
-      <c r="AE17" s="20"/>
+      <c r="AE17" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19"/>
@@ -2440,23 +2405,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:AE1"/>
+    <mergeCell ref="X4:AD4"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="Q4:W4"/>
+    <mergeCell ref="C8:P8"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Z13:AD13"/>
+    <mergeCell ref="Q10:AD10"/>
+    <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="U17:Y17"/>
     <mergeCell ref="Q9:AD9"/>
     <mergeCell ref="W12:Z12"/>
     <mergeCell ref="T14:Y14"/>
     <mergeCell ref="Q15:T15"/>
     <mergeCell ref="T16:Y16"/>
-    <mergeCell ref="C8:P8"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Z13:AD13"/>
-    <mergeCell ref="Q10:AD10"/>
-    <mergeCell ref="AE4:AE7"/>
-    <mergeCell ref="B1:AE1"/>
-    <mergeCell ref="X4:AD4"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="Q4:W4"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Daemon už ohlašuje svoje crashe serveru. Infrastruktura pro tvoření lokálních logů a odesílání jich na server vytvořena viz LocalLogManipulator
</commit_message>
<xml_diff>
--- a/timeline/2M Project Timeline.xlsx
+++ b/timeline/2M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4F47DA-26AC-49C0-BFBD-33811E4AF066}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D0DC9-66A7-41F2-83F7-DA440FFE40E4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -537,38 +537,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -822,7 +822,7 @@
   <dimension ref="B1:AJ125"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE16" sqref="AE16"/>
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -836,91 +836,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="24">
         <v>43171</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="32" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="30" t="s">
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="27" t="s">
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="30" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -1041,7 +1041,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="27"/>
+      <c r="AE5" s="30"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1160,7 +1160,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="27"/>
+      <c r="AE6" s="30"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1278,7 +1278,7 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43198</v>
       </c>
-      <c r="AE7" s="28"/>
+      <c r="AE7" s="31"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
@@ -1334,22 +1334,22 @@
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
       <c r="AE9" s="21" t="s">
         <v>6</v>
       </c>
@@ -1372,22 +1372,22 @@
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="25" t="s">
+      <c r="Q10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="25"/>
-      <c r="AD10" s="25"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
       <c r="AE10" s="20"/>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1408,12 +1408,12 @@
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
       <c r="W11" s="5"/>
@@ -1450,17 +1450,19 @@
       <c r="T12" s="6"/>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="22" t="s">
+      <c r="W12" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="20"/>
+      <c r="AE12" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
@@ -1489,13 +1491,13 @@
       <c r="W13" s="5"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="23" t="s">
+      <c r="Z13" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
       <c r="AE13" s="20"/>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1519,14 +1521,14 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="6"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="24" t="s">
+      <c r="T14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
       <c r="Z14" s="6"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="6"/>
@@ -1552,12 +1554,12 @@
       <c r="N15" s="6"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="22" t="s">
+      <c r="Q15" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
@@ -1593,14 +1595,14 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="6"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="25" t="s">
+      <c r="T16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="25"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="25"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
       <c r="Z16" s="6"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="6"/>
@@ -1630,13 +1632,13 @@
       <c r="R17" s="6"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="22" t="s">
+      <c r="U17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
       <c r="Z17" s="6"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="6"/>
@@ -2405,23 +2407,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="U17:Y17"/>
+    <mergeCell ref="Q9:AD9"/>
+    <mergeCell ref="W12:Z12"/>
+    <mergeCell ref="T14:Y14"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="T16:Y16"/>
+    <mergeCell ref="C8:P8"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Z13:AD13"/>
+    <mergeCell ref="Q10:AD10"/>
+    <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="B1:AE1"/>
     <mergeCell ref="X4:AD4"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="J4:P4"/>
     <mergeCell ref="Q4:W4"/>
-    <mergeCell ref="C8:P8"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Z13:AD13"/>
-    <mergeCell ref="Q10:AD10"/>
-    <mergeCell ref="AE4:AE7"/>
-    <mergeCell ref="U17:Y17"/>
-    <mergeCell ref="Q9:AD9"/>
-    <mergeCell ref="W12:Z12"/>
-    <mergeCell ref="T14:Y14"/>
-    <mergeCell ref="Q15:T15"/>
-    <mergeCell ref="T16:Y16"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Daemon komunikuje pomocí pipe s DS, umožňuje spoštěť dostat se ze sandboxu DS nedoděláno, víc logování
</commit_message>
<xml_diff>
--- a/timeline/2M Project Timeline.xlsx
+++ b/timeline/2M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D0DC9-66A7-41F2-83F7-DA440FFE40E4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222DCB98-B4AF-4FD2-8510-97A4073E6DAF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -537,6 +537,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -548,27 +569,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -822,7 +822,7 @@
   <dimension ref="B1:AJ125"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+      <selection activeCell="AH10" sqref="AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -836,91 +836,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="31">
         <v>43171</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="23" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="25" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="23" t="s">
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="30" t="s">
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -1041,7 +1041,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="30"/>
+      <c r="AE5" s="27"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1160,7 +1160,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="30"/>
+      <c r="AE6" s="27"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1278,7 +1278,7 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43198</v>
       </c>
-      <c r="AE7" s="31"/>
+      <c r="AE7" s="28"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
@@ -1334,25 +1334,23 @@
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="28"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28"/>
-      <c r="AE9" s="21" t="s">
-        <v>6</v>
-      </c>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="23"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="21"/>
     </row>
     <row r="10" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
@@ -1372,22 +1370,22 @@
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="29" t="s">
+      <c r="Q10" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
-      <c r="AB10" s="29"/>
-      <c r="AC10" s="29"/>
-      <c r="AD10" s="29"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="25"/>
       <c r="AE10" s="20"/>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1408,12 +1406,12 @@
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="27" t="s">
+      <c r="Q11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
       <c r="W11" s="5"/>
@@ -1450,12 +1448,12 @@
       <c r="T12" s="6"/>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="32" t="s">
+      <c r="W12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="32"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="5"/>
@@ -1491,13 +1489,13 @@
       <c r="W13" s="5"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="28" t="s">
+      <c r="Z13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="28"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
       <c r="AE13" s="20"/>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1521,14 +1519,14 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="6"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="27" t="s">
+      <c r="T14" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
       <c r="Z14" s="6"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="6"/>
@@ -1554,12 +1552,12 @@
       <c r="N15" s="6"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="32" t="s">
+      <c r="Q15" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
@@ -1595,14 +1593,14 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="6"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="29" t="s">
+      <c r="T16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
       <c r="Z16" s="6"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="6"/>
@@ -1632,13 +1630,13 @@
       <c r="R17" s="6"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="32" t="s">
+      <c r="U17" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="32"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
       <c r="Z17" s="6"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="6"/>
@@ -2407,30 +2405,30 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:AE1"/>
+    <mergeCell ref="X4:AD4"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="Q4:W4"/>
+    <mergeCell ref="C8:P8"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Z13:AD13"/>
+    <mergeCell ref="Q10:AD10"/>
+    <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="U17:Y17"/>
     <mergeCell ref="Q9:AD9"/>
     <mergeCell ref="W12:Z12"/>
     <mergeCell ref="T14:Y14"/>
     <mergeCell ref="Q15:T15"/>
     <mergeCell ref="T16:Y16"/>
-    <mergeCell ref="C8:P8"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Z13:AD13"/>
-    <mergeCell ref="Q10:AD10"/>
-    <mergeCell ref="AE4:AE7"/>
-    <mergeCell ref="B1:AE1"/>
-    <mergeCell ref="X4:AD4"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="Q4:W4"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C$7=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="9">
+  <dataValidations count="9">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline in this worksheet. Enter Start Date in cell C2 and other details starting in cell B4" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in cell at right" sqref="B2" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this cell" sqref="C2:E2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>

</xml_diff>

<commit_message>
Update timelajny. Novej kontroler připravenej pro smart fetchování
</commit_message>
<xml_diff>
--- a/timeline/2M Project Timeline.xlsx
+++ b/timeline/2M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222DCB98-B4AF-4FD2-8510-97A4073E6DAF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FC6C32-D894-46FC-BC85-F4C733E40B45}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>Dokončeno</t>
+  </si>
+  <si>
+    <t>Lukáš Dokončeno Rambo 50%</t>
+  </si>
+  <si>
+    <t>Nedokončeno</t>
   </si>
 </sst>
 </file>
@@ -537,38 +543,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -822,7 +828,7 @@
   <dimension ref="B1:AJ125"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -836,91 +842,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="24">
         <v>43171</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="32" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="30" t="s">
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="27" t="s">
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="30" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -1041,7 +1047,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="27"/>
+      <c r="AE5" s="30"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1160,7 +1166,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="27"/>
+      <c r="AE6" s="30"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1278,7 +1284,7 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43198</v>
       </c>
-      <c r="AE7" s="28"/>
+      <c r="AE7" s="31"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
@@ -1314,7 +1320,9 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="5"/>
       <c r="AD8" s="6"/>
-      <c r="AE8" s="20"/>
+      <c r="AE8" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
@@ -1334,23 +1342,25 @@
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="21"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="21" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
@@ -1370,23 +1380,25 @@
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="25" t="s">
+      <c r="Q10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="25"/>
-      <c r="AD10" s="25"/>
-      <c r="AE10" s="20"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
@@ -1406,12 +1418,12 @@
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
       <c r="U11" s="5"/>
       <c r="V11" s="6"/>
       <c r="W11" s="5"/>
@@ -1422,7 +1434,9 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="5"/>
       <c r="AD11" s="6"/>
-      <c r="AE11" s="20"/>
+      <c r="AE11" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
@@ -1448,12 +1462,12 @@
       <c r="T12" s="6"/>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="22" t="s">
+      <c r="W12" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="5"/>
@@ -1489,14 +1503,16 @@
       <c r="W13" s="5"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="23" t="s">
+      <c r="Z13" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="20"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
@@ -1519,20 +1535,22 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="6"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="24" t="s">
+      <c r="T14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
       <c r="Z14" s="6"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="6"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="6"/>
-      <c r="AE14" s="20"/>
+      <c r="AE14" s="21" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
@@ -1552,12 +1570,12 @@
       <c r="N15" s="6"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="22" t="s">
+      <c r="Q15" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
@@ -1593,20 +1611,22 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="6"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="25" t="s">
+      <c r="T16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="25"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="25"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
       <c r="Z16" s="6"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="6"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="6"/>
-      <c r="AE16" s="20"/>
+      <c r="AE16" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="2:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
@@ -1630,13 +1650,13 @@
       <c r="R17" s="6"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="22" t="s">
+      <c r="U17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
       <c r="Z17" s="6"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="6"/>
@@ -2405,23 +2425,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="U17:Y17"/>
+    <mergeCell ref="Q9:AD9"/>
+    <mergeCell ref="W12:Z12"/>
+    <mergeCell ref="T14:Y14"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="T16:Y16"/>
+    <mergeCell ref="C8:P8"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Z13:AD13"/>
+    <mergeCell ref="Q10:AD10"/>
+    <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="B1:AE1"/>
     <mergeCell ref="X4:AD4"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="J4:P4"/>
     <mergeCell ref="Q4:W4"/>
-    <mergeCell ref="C8:P8"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Z13:AD13"/>
-    <mergeCell ref="Q10:AD10"/>
-    <mergeCell ref="AE4:AE7"/>
-    <mergeCell ref="U17:Y17"/>
-    <mergeCell ref="Q9:AD9"/>
-    <mergeCell ref="W12:Z12"/>
-    <mergeCell ref="T14:Y14"/>
-    <mergeCell ref="Q15:T15"/>
-    <mergeCell ref="T16:Y16"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>